<commit_message>
booking part done done✅
</commit_message>
<xml_diff>
--- a/Appointment/doctor_appointments.xlsx
+++ b/Appointment/doctor_appointments.xlsx
@@ -476,11 +476,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ajeet12s3</t>
+          <t>abcded</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4262</v>
+        <v>4275</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -494,12 +494,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>2024-09-03</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>08:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>